<commit_message>
Integrate parent document retriever
</commit_message>
<xml_diff>
--- a/data/data_additional.xlsx
+++ b/data/data_additional.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/Final year (4th)/Dự án CNTT/Thu thập dữ liệu/Dữ liệu đã lọc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDTU\Year_4_Semester1\Dự án\Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7815B24D-44A5-5347-B5E4-6C4CBDD662B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1920AD61-6E30-45A6-9780-DA61D878C43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{588A6C13-E89E-6648-9010-D1D416D97C0B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{588A6C13-E89E-6648-9010-D1D416D97C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -60,9 +59,6 @@
 Sài Gòn (Thành phố Hồ Chí Minh) là thành phố lớn nhất Việt Nam và là một trong những điểm đến du lịch nổi tiếng nhất Đông Nam Á. Nơi đây thu hút du khách bởi sự năng động, hiện đại, giao thoa giữa văn hóa truyền thống và hiện đại, cùng với những địa điểm tham quan hấp dẫn, ẩm thực phong phú và con người thân thiện. Sài Gòn có rất nhiều điểm du lịch như Thảo Cầm Viên, Nhà thờ Đức Bà, Bến Nhà Rồng, Dinh Độc Lập, Chợ Bến Thành… Để di chuyển nhanh chóng giữa các địa điểm mà không phải lo về việc tìm tuyến đường thuận tiện nhất thì sử dụng dịch vụ taxi Sài Gòn là điều hoàn toàn đúng đắn. Sử dụng taxi Sài Gòn là giải pháp giúp bạn không cần phải lo lắng về việc tìm chỗ đỗ xe, đặc biệt là ở những khu vực trung tâm thành phố. Các hãng taxi uy tín tại Sài Gòn đều có đội xe hiện đại, được bảo dưỡng định kỳ và trang bị đầy đủ tiện nghi an toàn.
 Ngoài ra, ở Sài Gòn, bạn có thể dễ dàng đặt dịch vụ taxi đưa đón sân bay đáp ứng được nhu cầu di chuyển sau chuyến bay dài hoặc có mặt tại sân bay đúng giờ để làm thủ tục.
 Top 13 hãng taxi Sài Gòn uy tín, chuyên nghiệp nhất1. Taxi VinasunTổng đài taxi Taxi Vinasun: (028) 38 27 27 27Vinasun Taxi luôn chú trọng vào chất lượng dịch vụ, đảm bảo mang đến cho khách hàng những trải nghiệm tốt nhất. Các tài xế đều được đào tạo bài bản, có kinh nghiệm lái xe lâu năm và luôn phục vụ khách hàng với thái độ thân thiện, nhiệt tình.Vinasun Taxi hoạt động 24/24, 7 ngày trong tuần, đáp ứng nhu cầu di chuyển của khách hàng mọi lúc mọi nơi.@shutterstock2. Taxi Mai LinhTổng đài Taxi Mai Linh: Tổng đài 1055Với phương châm "An toàn - Chất lượng - Uy tín", Taxi Mai Linh đã không ngừng phát triển và khẳng định vị thế của mình trên thị trường, trở thành người bạn đồng hành tin cậy của hàng triệu khách hàng trên khắp cả nước. Taxi Mai Linh áp dụng mức giá cạnh tranh cho các dịch vụ của mình. Giá cước được niêm yết rõ ràng trên website và ứng dụng, giúp khách hàng dễ dàng tra cứu và so sánh.Taxi Mai Linh có ứng dụng đặt xe tiện lợi, giúp khách hàng dễ dàng đặt xe mọi lúc mọi nơi.@shutterstock3. Taxi Xanh SMTổng đài taxi Xanh SM: 1900 2088Được thành lập với mục đích mang lại sự tiện lợi và an toàn cho khách hàng, Taxi Xanh SM đã nhanh chóng khẳng định vị thế của mình trong ngành công nghiệp dịch vụ đi lại bằng những dòng xe hiện đại và đội ngũ lái xe chuyên nghiệp. Taxi Xanh SM sở hữu một flotilla xe đa dạng từ sedan, SUV đến xe hơi cao cấp, đảm bảo đáp ứng mọi nhu cầu đi lại của khách hàng từ cá nhân đến công ty.Taxi Xanh SM luôn lắng nghe và cải thiện dịch vụ dựa trên phản hồi của khách hàng, đảm bảo sự hài lòng cao nhất. @Taxi Xanh SM4. Gocar TaxiTổng đài taxi Gocar: 1900636252Cuối năm 2021, Gojek, một trong những nền tảng công nghệ hàng đầu tại Đông Nam Á với các dịch vụ đa lĩnh vực theo yêu cầu, đã công bố một bước mở rộng quan trọng: dịch vụ gọi xe ô tô công nghệ GoCar chính thức có mặt tại Thành phố Hồ Chí Minh. Đây là một phần trong chiến lược mở rộng của Gojek, nhằm mang đến cho người dùng tại thành phố này trải nghiệm mới với dòng sản phẩm GoCar Protect. Điều đã mang lại sự thuận tiện và tiện ích cho người dùng khi di chuyển trong đô thị sôi động như TP.HCM.Gocar Taxi được rất nhiều người dân Sài Gòn ưa chuộng.@Taxi Gocar5. Grab Car TaxiTổng đài taxi Grab Car: 028 7108 7108Không cần lo về giá cả với GrabCar. Giá tiền cuốc xe được hiển thị ngay trên ứng dụng, bạn chỉ cần thanh toán đúng số tiền này và hoàn toàn yên tâm tận hưởng chuyến đi của mình. GrabCar không chỉ có bảo hiểm xuyên suốt cho tài xế trong suốt hành trình, mà còn có bảo hiểm dành cho hành khách, đảm bảo an toàn cho cả bạn và tài xế trong mỗi chuyến đi. Hầu hết các tài xế GrabCar đều có kinh nghiệm lái xe lâu năm, đảm bảo mang đến cho bạn dịch vụ tốt nhất và an toàn nhất.Với Grab Car an toàn là trên hết.@Grab car Taxi6. Taxi Sài Gòn G7Tổng đài taxi Sài Gòn G7: 028 38 16 16 16G7 Taxi hoạt động chủ yếu tại các quận trung tâm TP.HCM và đặc biệt là tại Sân bay Tân Sơn Nhất, nổi bật như một trong những hãng taxi chính phục vụ khách hàng tại cảng hàng không quốc tế này. G7 Taxi HCM tự hào là lựa chọn với mức giá cạnh tranh và chất lượng dịch vụ tốt, mang đến trải nghiệm xuất sắc cho mỗi hành trình của khách hàng, cam kết mang đến những giá trị tốt nhất cho khách hàng và các tài xế.G7 Taxi thường triển khai nhiều chương trình ưu đãi hấp dẫn.@Taxi G77. Vina TaxiTổng đài Vina taxi: 028 38 111 111Để đáp ứng nhu cầu của khách hàng một cách tốt nhất, từ đầu năm 2022 đến nay, Vinataxi liên tục nhập khẩu các dòng xe 4 chỗ và 7 chỗ mới như Innova, Avanza, Vios. Đội xe taxi màu vàng của Vinataxi không chỉ nổi bật mà còn đáp ứng các tiêu chí về sạch sẽ, phục vụ chu đáo và giá cả phải chăng. Đây luôn là lựa chọn hàng đầu của cá nhân và doanh nghiệp khi cần di chuyển trong TP.HCM và các tỉnh lân cận.Vinataxi tiếp tục thành công từ năm 2022 và được khách hàng tin tưởng.@Taxi Vina8. Taxi Sasco TravelTổng đài taxi Sasco Travel: 028 3547 0295Taxi Sasco Travel là một hãng taxi uy tín tại TP. Hồ Chí Minh, chuyên cung cấp dịch vụ đưa đón sân bay Tân Sơn Nhất và các sân bay lân cận. Sasco Travel đã khẳng định được vị thế của mình trên thị trường và trở thành đối tác tin cậy của nhiều hãng hàng không, khách sạn và công ty du lịch. Sasco Travel còn cung cấp dịch vụ đặt vé máy bay, khách sạn cho khách hàng, giúp khách hàng tiết kiệm thời gian và chi phí. Khách hàng có thể dễ dàng đặt xe qua tổng đài, website, ứng dụng hoặc trực tiếp tại các quầy dịch vụ của Sasco Travel tại sân bay.@Taxi Sasco Travel9. Hoàng Long Sài Gòn TaxiTổng đài Hoàng Long Sài Gòn taxi:(028) 38 68 68 68Vào ngày 10/08/2007, chính thức khai trương đoàn xe mang thương hiệu Taxi Sài Gòn Hoàng Long tại TP.HCM. Ban đầu, hoạt động hơn 300 xe taxi bao gồm Toyota Vios 4 chỗ và Toyota Innova 7 chỗ, các dòng xe Model 2007, phủ sóng tại 24 quận, huyện của thành phố. Đầu năm 2010, Công ty tiếp tục đáp ứng nhu cầu của người tiêu dùng bằng việc ra mắt thương hiệu taxi mới mang tên City Taxi. Đây là sự đổi mới của công ty với dòng xe Toyota 4 chỗ, nhằm cung cấp cho khách hàng một lựa chọn tiện lợi và đáng tin cậy trong việc di chuyển trong thành phố.Taxi Hoàng Long Sài Gòn luôn được nhiều khách hàng lựa chọn@Taxi Hoàng Long Sài Gòn10. Taxi Bình PhátTổng đài Taxi Bình Phát: 028.38.75.27.20Taxi Bình Phát cam kết mang đến cho khách hàng dịch vụ di chuyển hoàn hảo. Hãng luôn chú trọng đến sự an toàn của hành khách bằng việc bảo dưỡng định kỳ xe và đào tạo đội ngũ tài xế chuyên nghiệp, giàu kinh nghiệm. Mỗi hành trình đều được hãng đảm bảo tuyệt đối về mặt an toàn, giúp khách hàng yên tâm trong suốt quá trình di chuyển.Với dịch vụ hiện đại, uy tín cùng thái độ phục vụ chuyên nghiệp, Taxi Bình Phát luôn được lựa chọn nhiều nhất. @ Taxi Bình Phát11. Sài Gòn TaxiTổng đài Sài Gòn Taxi: (0251) 36 36 36 36Sài Gòn Taxi, với thương hiệu "Taxi Giá rẻ" đã từng được lòng người dân TP Hồ Chí Minh trong một thời gian dài nhờ tính tiện lợi và đáng tin cậy, giờ đây đã trở lại với một sự đổi mới rõ rệt. Công ty đã quyết định đưa vào dịch vụ những dòng xe mới như Xpander và Kia Seltos, nhằm cải thiện trải nghiệm của khách hàng. Điều này không chỉ mở rộng phạm vi và chất lượng dịch vụ mà còn thể hiện cam kết của công ty trong việc đáp ứng nhu cầu di chuyển của người dân và du khách một cách hiệu quả và tiện lợi nhất.Taxi Sài Gòn với những mẫu xe đời mới, phục vụ chuyên nghiệp luôn mang đến cho khách hàng sự an toàn tuyệt đối. @Taxi Sài Gòn12. Taxi Gia Đình ViệtTổng đài Taxi Gia Đình Việt: 09.3355.3999Đội ngũ tài xế của Taxi Gia Đình Việt không chỉ có kinh nghiệm lâu năm mà còn luôn nhiệt tình và chu đáo với mỗi chuyến đi của khách hàng. Họ luôn sẵn sàng hỗ trợ và đưa ra các lựa chọn tối ưu để khách hàng có trải nghiệm di chuyển thoải mái và an toàn nhất.Taxi Gia Đình Việt luôn được bảo dưỡng để đảm bảo an toàn, thoải mái cho hành khách. @Taxi Gia Đình Việt13. Taxi 27-7Tổng đài Taxi 27-7: 028 5427 2727Taxi 27-7 là một trong những lựa chọn hàng đầu của du khách khi đến thăm Sài Gòn. Với hơn một thập kỷ hoạt động trong ngành dịch vụ taxi, hãng đã ghi dấu ấn với khách hàng nhờ vào sự kết hợp giữa chất lượng dịch vụ cao và đội ngũ tài xế chuyên nghiệp, thân thiện.Với thái độ phục vụ chuyên nghiệp, taxi 27-7 là lựa chọn của nhiều người khi đến Sài Gòn. @Taxi 27-7Giá cước taxi Sài Gòn để bạn tham khảoGiá cước có thể thay đổi tùy theo thời điểm, khu vực và loại xe bạn chọn. Nên tham khảo thông tin giá cước mới nhất trên website hoặc ứng dụng của từng hãng trước khi đặt xe.Giá mở cửa: 8.000 - 17.000 VNDGiá các km tiếp theo: 13.000 - 17.000 VND/ kmGiá từ mốc 31km trở lên: 10.500 - 12.500 VND/ kmKinh nghiệm đặt taxi Sài Gòn bạn nên biếtCách đặt taxi Sài GònSử dụng ứng dụng: các ứng dụng của các hãng như Grab, Gojek hoặc Vinasun, Mai Linh Taxi có thể giúp bạn đặt xe nhanh chóng và thuận tiện. Vào các khung giờ cao điểm hoặc khi bạn có lịch trình cụ thể, nên đặt xe trước ít nhất vài phút để đảm bảo có xe sẵn sàng khi bạn cần.Bắt taxi trực tiếp: Chọn điểm đón xe taxi tại những nơi an toàn, có ánh sáng và dễ dàng để tài xế có thể tiếp cận và đón bạn một cách thuận tiện, đảm bảo an toàn.Lưu ý khi sử dụng taxi Sài Gòn để an toàn, tiện lợiNếu bạn đón xe trực tiếp từ đường phố, biết cách đàm phán giá cước trước khi lên xe để tránh bất ngờ về giá.Trong suốt hành trình luôn kiểm tra và xác nhận địa điểm đón và đích đến cho tài xế, đảm bảo rằng họ sẽ đưa bạn đến đúng địa điểm mà không bị lạc đường.Sau khi đến nơi, hãy kiểm tra kỹ hành lý và trả cước đúng với số tiền đã thỏa thuận trước đó.</t>
-  </si>
-  <si>
-    <t>Hồ Chí Minh</t>
   </si>
   <si>
     <t>Transport</t>
@@ -1296,12 +1292,15 @@
     <t xml:space="preserve">Tập tài liệu này tổng hợp các nguồn thông tin du lịch đa dạng về Việt Nam, tập trung chính vào TP.HCM và Đà Nẵng. Nguồn tham khảo bao gồm các trang chính thức của cơ quan du lịch và chính quyền (như Vietnam.travel, Danang Fantasticity, danang.gov.vn), cùng với các nền tảng thương mại và dịch vụ đặt chỗ (như Traveloka, Klook, VinWonders) và các blog chia sẻ kinh nghiệm du lịch cá nhân.
 </t>
   </si>
+  <si>
+    <t>Thành phố Hồ Chí Minh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1702,13 +1701,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302DAE12-D407-9548-9B20-99E47C7FA2D2}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17.399999999999999">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="409.6">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1733,426 +1732,426 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="409.6">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="409.6">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="409.6">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="409.6">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="409.6">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="409.6">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="409.6">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="409.6">
+      <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="409.6">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="409.6">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="409.6">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="409.6">
+      <c r="A14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="409.6">
+      <c r="A15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="409.6">
+      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="409.6">
+      <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="409.6">
+      <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="409.6">
+      <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="409.6">
+      <c r="A20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="409.6">
+      <c r="A21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="409.6">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="409.6">
+      <c r="A23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="409.6">
+      <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="409.6">
+      <c r="A25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="409.6">
+      <c r="A26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="409.6">
+      <c r="A27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="409.6">
+      <c r="A28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="E28" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="409.6">
+      <c r="A29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>